<commit_message>
vdw updates -- we are no longer looking at vdw model
</commit_message>
<xml_diff>
--- a/modsel/vdWTest_Scipy/vdW_python_check.xlsx
+++ b/modsel/vdWTest_Scipy/vdW_python_check.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bridgettebefort/Dowling-Maginn-Lab/DowlingLab/extractive-distillation2/modsel/vdWTest_Scipy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EC7790-0CB1-3A48-ADBC-3576ABF075A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E45C4E8-DFB7-5148-8FD1-216A3099E8F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="0" windowWidth="10000" windowHeight="18000" activeTab="1" xr2:uid="{8C003C96-9324-4741-A374-113BA67ED0A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{8C003C96-9324-4741-A374-113BA67ED0A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Point1, different BIP" sheetId="2" r:id="rId1"/>

</xml_diff>